<commit_message>
Created more testdata & implemented Settings class
</commit_message>
<xml_diff>
--- a/tests/Testdata.xlsx
+++ b/tests/Testdata.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maart\Documents\Syntra\groepswerk-1\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BD5A37-888D-4C2D-8B5B-A41E80B6B863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B5C05ED-A69B-4A2C-93AC-36E567BC2127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12675" yWindow="3015" windowWidth="16215" windowHeight="11385" tabRatio="844" firstSheet="7" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Club" sheetId="1" r:id="rId1"/>
-    <sheet name="Match" sheetId="2" r:id="rId2"/>
-    <sheet name="Matchday" sheetId="3" r:id="rId3"/>
+    <sheet name="Season" sheetId="15" r:id="rId1"/>
+    <sheet name="League" sheetId="8" r:id="rId2"/>
+    <sheet name="Competition" sheetId="6" r:id="rId3"/>
+    <sheet name="Series" sheetId="16" r:id="rId4"/>
+    <sheet name="Matchday" sheetId="3" r:id="rId5"/>
+    <sheet name="Player" sheetId="10" r:id="rId6"/>
+    <sheet name="Club" sheetId="1" r:id="rId7"/>
+    <sheet name="Clubcontact" sheetId="5" r:id="rId8"/>
+    <sheet name="Team" sheetId="4" r:id="rId9"/>
+    <sheet name="Registration" sheetId="13" r:id="rId10"/>
+    <sheet name="Referee" sheetId="11" r:id="rId11"/>
+    <sheet name="Location" sheetId="9" r:id="rId12"/>
+    <sheet name="Refereedistance" sheetId="12" r:id="rId13"/>
+    <sheet name="Match" sheetId="2" r:id="rId14"/>
+    <sheet name="Injury" sheetId="7" r:id="rId15"/>
+    <sheet name="Sanction" sheetId="14" r:id="rId16"/>
   </sheets>
   <definedNames>
-    <definedName name="club" localSheetId="0">Club!$A$1:$P$3</definedName>
-    <definedName name="match" localSheetId="1">Match!$A$1:$P$2</definedName>
-    <definedName name="matchday" localSheetId="2">Matchday!$A$1:$D$2</definedName>
+    <definedName name="club" localSheetId="6">Club!$A$1:$P$3</definedName>
+    <definedName name="match" localSheetId="13">Match!$A$1:$P$2</definedName>
+    <definedName name="matchday" localSheetId="4">Matchday!$A$1:$D$2</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -86,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="110">
   <si>
     <t>id</t>
   </si>
@@ -208,15 +221,6 @@
     <t>Matchday 5</t>
   </si>
   <si>
-    <t>Matchday 13</t>
-  </si>
-  <si>
-    <t>Matchday 20</t>
-  </si>
-  <si>
-    <t>Matchday 25</t>
-  </si>
-  <si>
     <t>toto</t>
   </si>
   <si>
@@ -230,16 +234,217 @@
   </si>
   <si>
     <t>true</t>
+  </si>
+  <si>
+    <t>display_name</t>
+  </si>
+  <si>
+    <t>home_color_1</t>
+  </si>
+  <si>
+    <t>home_color_2</t>
+  </si>
+  <si>
+    <t>home_color_3</t>
+  </si>
+  <si>
+    <t>away_color_1</t>
+  </si>
+  <si>
+    <t>away_color_2</t>
+  </si>
+  <si>
+    <t>away_color_3</t>
+  </si>
+  <si>
+    <t>alt_color_1</t>
+  </si>
+  <si>
+    <t>alt_color_2</t>
+  </si>
+  <si>
+    <t>alt_color_3</t>
+  </si>
+  <si>
+    <t>club_id</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>middle_names</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>competition_type</t>
+  </si>
+  <si>
+    <t>league_id</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>match_id</t>
+  </si>
+  <si>
+    <t>player_id</t>
+  </si>
+  <si>
+    <t>season_id</t>
+  </si>
+  <si>
+    <t>date_of_birth</t>
+  </si>
+  <si>
+    <t>country_of_birth</t>
+  </si>
+  <si>
+    <t>national_identification</t>
+  </si>
+  <si>
+    <t>identification</t>
+  </si>
+  <si>
+    <t>city_of_birth</t>
+  </si>
+  <si>
+    <t>start_date</t>
+  </si>
+  <si>
+    <t>end_date</t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t>team_id</t>
+  </si>
+  <si>
+    <t>sanction_type</t>
+  </si>
+  <si>
+    <t>report</t>
+  </si>
+  <si>
+    <t>competition_id</t>
+  </si>
+  <si>
+    <t>2021-2022</t>
+  </si>
+  <si>
+    <t>HZVB</t>
+  </si>
+  <si>
+    <t>Eerste klasse</t>
+  </si>
+  <si>
+    <t>competitie</t>
+  </si>
+  <si>
+    <t>has_secondary_score</t>
+  </si>
+  <si>
+    <t>Week 1</t>
+  </si>
+  <si>
+    <t>Matchday 2</t>
+  </si>
+  <si>
+    <t>Matchday 3</t>
+  </si>
+  <si>
+    <t>Matchday 4</t>
+  </si>
+  <si>
+    <t>Maarten</t>
+  </si>
+  <si>
+    <t>Vanhulst</t>
+  </si>
+  <si>
+    <t>Koekoesstraat</t>
+  </si>
+  <si>
+    <t>Melle</t>
+  </si>
+  <si>
+    <t>BEL</t>
+  </si>
+  <si>
+    <t>0032495123456</t>
+  </si>
+  <si>
+    <t>Schalkse_ruiter@hetemail.com</t>
+  </si>
+  <si>
+    <t>Big Boss</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Yves</t>
+  </si>
+  <si>
+    <t>Vindevogel</t>
+  </si>
+  <si>
+    <t>Ergens</t>
+  </si>
+  <si>
+    <t>Anders</t>
+  </si>
+  <si>
+    <t>Ginder</t>
+  </si>
+  <si>
+    <t>Yves@vindevogel.com</t>
+  </si>
+  <si>
+    <t>Place2B</t>
+  </si>
+  <si>
+    <t>Een</t>
+  </si>
+  <si>
+    <t>Stad</t>
+  </si>
+  <si>
+    <t>P2B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -265,7 +470,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
@@ -285,6 +490,9 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -303,15 +511,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="matchday" connectionId="3" xr16:uid="{00000000-0016-0000-0200-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="club" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="match" connectionId="2" xr16:uid="{00000000-0016-0000-0100-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="matchday" connectionId="3" xr16:uid="{00000000-0016-0000-0200-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -634,274 +842,389 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E683638F-F1C1-4599-81AC-E5374DFB5099}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2">
-        <v>3000</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="B2" t="s">
         <v>44</v>
       </c>
-      <c r="I2">
-        <v>112</v>
-      </c>
-      <c r="L2" t="s">
-        <v>45</v>
-      </c>
-      <c r="P2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3">
-        <v>3000</v>
-      </c>
-      <c r="G3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I3">
-        <v>112</v>
-      </c>
-      <c r="L3" t="s">
-        <v>45</v>
-      </c>
-      <c r="P3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4">
-        <v>3000</v>
-      </c>
-      <c r="G4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4">
-        <v>112</v>
-      </c>
-      <c r="L4" t="s">
-        <v>45</v>
-      </c>
-      <c r="P4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5">
-        <v>3000</v>
-      </c>
-      <c r="G5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5">
-        <v>112</v>
-      </c>
-      <c r="L5" t="s">
-        <v>45</v>
-      </c>
-      <c r="P5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6">
-        <v>3000</v>
-      </c>
-      <c r="G6" t="s">
-        <v>44</v>
-      </c>
-      <c r="I6">
-        <v>112</v>
-      </c>
-      <c r="L6" t="s">
-        <v>45</v>
-      </c>
-      <c r="P6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="7">
+        <v>44440</v>
+      </c>
+      <c r="E2" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B1B2D5-55BB-48DB-83FC-309ACE7D30C6}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="7">
+        <v>44197</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA18B3A-94C1-4672-AA14-799856947F85}">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" t="s">
+        <v>70</v>
+      </c>
+      <c r="L1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2">
+        <v>1000</v>
+      </c>
+      <c r="H2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J2" s="7">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M2">
+        <v>1234567890</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2">
+        <v>123</v>
+      </c>
+      <c r="S2">
+        <v>456</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B0C57A3-81B6-4142-9F59-2AB94E027BA2}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2">
+        <v>9999</v>
+      </c>
+      <c r="F2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2">
+        <v>987654321</v>
+      </c>
+      <c r="K2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6AD5058-75B9-48E8-8793-D4E58A8C4C17}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P55"/>
   <sheetViews>
@@ -996,16 +1319,16 @@
         <v>2</v>
       </c>
       <c r="H2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="J2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L2" s="6">
         <v>5</v>
@@ -1034,16 +1357,16 @@
         <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="J3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L3" s="5">
         <v>14</v>
@@ -1072,16 +1395,16 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="J4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L4" s="5">
         <v>17</v>
@@ -1110,16 +1433,16 @@
         <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="J5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L5" s="5">
         <v>19</v>
@@ -1148,16 +1471,16 @@
         <v>2</v>
       </c>
       <c r="H6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="J6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L6" s="5">
         <v>2</v>
@@ -1371,12 +1694,220 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FC4E959-00D3-458F-BF2D-9646A0721B6E}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBCB9800-CB31-47F8-8ECE-6977E29CEA9C}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{116552E2-6160-4EA3-BCF2-88509FC3CA50}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C7701A-504D-4EA5-97B9-0D3E99095BD0}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{944857E9-3A88-403D-AA82-6F2999790571}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1420,7 +1951,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1434,7 +1965,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -1448,7 +1979,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -1462,16 +1993,663 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF13CEB0-4264-473F-B036-B572A63BFA30}">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>68</v>
+      </c>
+      <c r="R1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2">
+        <v>9090</v>
+      </c>
+      <c r="H2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J2" s="7">
+        <v>32380</v>
+      </c>
+      <c r="K2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q2">
+        <v>88082537701</v>
+      </c>
+      <c r="R2">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2">
+        <v>3000</v>
+      </c>
+      <c r="G2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2">
+        <v>112</v>
+      </c>
+      <c r="L2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3">
+        <v>3000</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3">
+        <v>112</v>
+      </c>
+      <c r="L3" t="s">
+        <v>42</v>
+      </c>
+      <c r="P3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4">
+        <v>3000</v>
+      </c>
+      <c r="G4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4">
+        <v>112</v>
+      </c>
+      <c r="L4" t="s">
+        <v>42</v>
+      </c>
+      <c r="P4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5">
+        <v>3000</v>
+      </c>
+      <c r="G5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5">
+        <v>112</v>
+      </c>
+      <c r="L5" t="s">
+        <v>42</v>
+      </c>
+      <c r="P5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6">
+        <v>3000</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6">
+        <v>112</v>
+      </c>
+      <c r="L6" t="s">
+        <v>42</v>
+      </c>
+      <c r="P6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25D117DD-87F5-4F42-8DF4-07E072A9DF7E}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J2" t="s">
+        <v>94</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6057B729-1C87-47B9-B9A8-A95F7353F366}">
+  <dimension ref="A1:M6"/>
+  <sheetViews>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" t="s">
+        <v>96</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" t="s">
+        <v>97</v>
+      </c>
+      <c r="M3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4" t="s">
+        <v>98</v>
+      </c>
+      <c r="M4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" t="s">
+        <v>99</v>
+      </c>
+      <c r="M5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>99</v>
+      </c>
+      <c r="G6" t="s">
+        <v>95</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
import testdata by for loops
</commit_message>
<xml_diff>
--- a/tests/Testdata.xlsx
+++ b/tests/Testdata.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maart\Documents\Syntra\groepswerk-1\tests\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B5C05ED-A69B-4A2C-93AC-36E567BC2127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12675" yWindow="3015" windowWidth="16215" windowHeight="11385" tabRatio="844" firstSheet="7" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12675" yWindow="3015" windowWidth="16215" windowHeight="11385" tabRatio="844" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Season" sheetId="15" r:id="rId1"/>
@@ -40,8 +34,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="club" type="6" refreshedVersion="3" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="club" type="6" refreshedVersion="3" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Datatables\club.csv" decimal="," thousands=" " comma="1">
       <textFields count="16">
         <textField/>
@@ -63,7 +57,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="match" type="6" refreshedVersion="3" background="1" saveData="1">
+  <connection id="2" name="match" type="6" refreshedVersion="3" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Datatables\match.csv" decimal="," thousands=" " comma="1">
       <textFields count="16">
         <textField/>
@@ -85,7 +79,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="matchday" type="6" refreshedVersion="3" background="1" saveData="1">
+  <connection id="3" name="matchday" type="6" refreshedVersion="3" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Datatables\matchday.csv" decimal="," thousands=" " comma="1">
       <textFields count="4">
         <textField/>
@@ -344,9 +338,6 @@
     <t>Eerste klasse</t>
   </si>
   <si>
-    <t>competitie</t>
-  </si>
-  <si>
     <t>has_secondary_score</t>
   </si>
   <si>
@@ -429,13 +420,16 @@
   </si>
   <si>
     <t>P2B</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -511,21 +505,21 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="matchday" connectionId="3" xr16:uid="{00000000-0016-0000-0200-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="matchday" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="club" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="club" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="match" connectionId="2" xr16:uid="{00000000-0016-0000-0100-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="match" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -563,9 +557,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -597,27 +591,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -649,27 +625,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -842,14 +800,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E683638F-F1C1-4599-81AC-E5374DFB5099}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
@@ -858,7 +816,7 @@
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -875,7 +833,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -896,19 +854,19 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B1B2D5-55BB-48DB-83FC-309ACE7D30C6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -931,7 +889,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -957,20 +915,20 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA18B3A-94C1-4672-AA14-799856947F85}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1029,39 +987,39 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" t="s">
         <v>100</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>101</v>
-      </c>
-      <c r="E2" t="s">
-        <v>102</v>
       </c>
       <c r="G2">
         <v>1000</v>
       </c>
       <c r="H2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J2" s="7">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
         <v>103</v>
-      </c>
-      <c r="I2" t="s">
-        <v>91</v>
-      </c>
-      <c r="J2" s="7">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
-        <v>104</v>
       </c>
       <c r="M2">
         <v>1234567890</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="R2">
         <v>123</v>
@@ -1076,19 +1034,19 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B0C57A3-81B6-4142-9F59-2AB94E027BA2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1132,30 +1090,30 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
         <v>106</v>
-      </c>
-      <c r="C2" t="s">
-        <v>107</v>
       </c>
       <c r="E2">
         <v>9999</v>
       </c>
       <c r="F2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H2">
         <v>987654321</v>
       </c>
       <c r="K2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1165,14 +1123,14 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6AD5058-75B9-48E8-8793-D4E58A8C4C17}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
@@ -1182,7 +1140,7 @@
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1202,7 +1160,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1225,14 +1183,14 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -1252,7 +1210,7 @@
     <col min="16" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1302,7 +1260,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1340,7 +1298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1378,7 +1336,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1416,7 +1374,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1454,7 +1412,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1492,199 +1450,199 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="B7" s="2"/>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="B8" s="2"/>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="B9" s="2"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="B10" s="2"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="B11" s="2"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="B12" s="2"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="B13" s="2"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="B15" s="2"/>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16">
       <c r="B16" s="2"/>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3">
       <c r="B17" s="2"/>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3">
       <c r="B18" s="2"/>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3">
       <c r="B19" s="2"/>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3">
       <c r="B20" s="2"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3">
       <c r="B21" s="2"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3">
       <c r="B22" s="2"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3">
       <c r="B23" s="2"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3">
       <c r="B24" s="2"/>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3">
       <c r="B25" s="2"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3">
       <c r="B26" s="2"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3">
       <c r="B27" s="2"/>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3">
       <c r="B28" s="2"/>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3">
       <c r="B29" s="2"/>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3">
       <c r="B30" s="2"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3">
       <c r="B31" s="2"/>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3">
       <c r="B32" s="2"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3">
       <c r="B33" s="2"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3">
       <c r="B34" s="2"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3">
       <c r="B35" s="2"/>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3">
       <c r="B36" s="2"/>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3">
       <c r="B37" s="2"/>
       <c r="C37" s="3"/>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3">
       <c r="B38" s="2"/>
       <c r="C38" s="3"/>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3">
       <c r="B39" s="2"/>
       <c r="C39" s="3"/>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3">
       <c r="B40" s="2"/>
       <c r="C40" s="3"/>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3">
       <c r="B41" s="2"/>
       <c r="C41" s="3"/>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3">
       <c r="B42" s="2"/>
       <c r="C42" s="3"/>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3">
       <c r="B43" s="2"/>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3">
       <c r="B44" s="2"/>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3">
       <c r="B45" s="2"/>
       <c r="C45" s="3"/>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3">
       <c r="B46" s="2"/>
       <c r="C46" s="3"/>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:3">
       <c r="B47" s="2"/>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:3">
       <c r="B48" s="2"/>
       <c r="C48" s="3"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3">
       <c r="B49" s="2"/>
       <c r="C49" s="3"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3">
       <c r="B50" s="2"/>
       <c r="C50" s="3"/>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3">
       <c r="B51" s="2"/>
       <c r="C51" s="3"/>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3">
       <c r="B52" s="2"/>
       <c r="C52" s="3"/>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3">
       <c r="B53" s="2"/>
       <c r="C53" s="3"/>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:3">
       <c r="B54" s="2"/>
       <c r="C54" s="3"/>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:3">
       <c r="B55" s="2"/>
       <c r="C55" s="3"/>
     </row>
@@ -1695,21 +1653,21 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FC4E959-00D3-458F-BF2D-9646A0721B6E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1729,16 +1687,16 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBCB9800-CB31-47F8-8ECE-6977E29CEA9C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1761,16 +1719,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{116552E2-6160-4EA3-BCF2-88509FC3CA50}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1781,7 +1739,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1798,14 +1756,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C7701A-504D-4EA5-97B9-0D3E99095BD0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -1814,7 +1772,7 @@
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1825,13 +1783,13 @@
         <v>60</v>
       </c>
       <c r="D1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1839,7 +1797,7 @@
         <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="D2" t="s">
         <v>43</v>
@@ -1854,14 +1812,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{944857E9-3A88-403D-AA82-6F2999790571}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
@@ -1869,7 +1827,7 @@
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1883,12 +1841,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1903,14 +1861,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
@@ -1918,7 +1876,7 @@
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1932,7 +1890,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1946,12 +1904,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1960,12 +1918,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -1974,12 +1932,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -1988,7 +1946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2009,14 +1967,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF13CEB0-4264-473F-B036-B572A63BFA30}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -2037,7 +1995,7 @@
     <col min="18" max="18" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2093,36 +2051,36 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" t="s">
         <v>87</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>88</v>
-      </c>
-      <c r="E2" t="s">
-        <v>89</v>
       </c>
       <c r="G2">
         <v>9090</v>
       </c>
       <c r="H2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J2" s="7">
         <v>32380</v>
       </c>
       <c r="K2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L2" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="O2" s="9" t="s">
         <v>92</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>93</v>
       </c>
       <c r="Q2">
         <v>88082537701</v>
@@ -2137,14 +2095,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
@@ -2162,7 +2120,7 @@
     <col min="16" max="16" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2212,7 +2170,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2241,7 +2199,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2270,7 +2228,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2299,7 +2257,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2328,7 +2286,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2357,46 +2315,46 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16">
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2">
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2">
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2">
       <c r="B20" s="1"/>
     </row>
   </sheetData>
@@ -2405,14 +2363,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25D117DD-87F5-4F42-8DF4-07E072A9DF7E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
@@ -2426,7 +2384,7 @@
     <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2461,24 +2419,24 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="G2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J2" t="s">
         <v>93</v>
-      </c>
-      <c r="G2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I2" t="s">
-        <v>88</v>
-      </c>
-      <c r="J2" t="s">
-        <v>94</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -2490,14 +2448,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6057B729-1C87-47B9-B9A8-A95F7353F366}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="18.140625" bestFit="1" customWidth="1"/>
@@ -2507,7 +2465,7 @@
     <col min="13" max="13" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2548,7 +2506,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2559,16 +2517,16 @@
         <v>33</v>
       </c>
       <c r="D2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" t="s">
         <v>95</v>
       </c>
-      <c r="G2" t="s">
-        <v>96</v>
-      </c>
       <c r="M2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2579,16 +2537,16 @@
         <v>34</v>
       </c>
       <c r="D3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G3" t="s">
         <v>96</v>
-      </c>
-      <c r="G3" t="s">
-        <v>97</v>
       </c>
       <c r="M3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2599,16 +2557,16 @@
         <v>35</v>
       </c>
       <c r="D4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G4" t="s">
         <v>97</v>
-      </c>
-      <c r="G4" t="s">
-        <v>98</v>
       </c>
       <c r="M4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2619,16 +2577,16 @@
         <v>36</v>
       </c>
       <c r="D5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" t="s">
         <v>98</v>
-      </c>
-      <c r="G5" t="s">
-        <v>99</v>
       </c>
       <c r="M5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2639,10 +2597,10 @@
         <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M6">
         <v>5</v>

</xml_diff>

<commit_message>
Bugfix: add_team.sql was empty & team_id in matches not in teams
</commit_message>
<xml_diff>
--- a/tests/Testdata.xlsx
+++ b/tests/Testdata.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maart\Documents\Syntra\groepswerk-1\tests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4874BE71-2BEC-44A3-BC27-3BE689F94685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12675" yWindow="3015" windowWidth="16215" windowHeight="11385" tabRatio="844" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="844" firstSheet="1" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Season" sheetId="15" r:id="rId1"/>
@@ -34,8 +40,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="club" type="6" refreshedVersion="3" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="club" type="6" refreshedVersion="3" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Datatables\club.csv" decimal="," thousands=" " comma="1">
       <textFields count="16">
         <textField/>
@@ -57,7 +63,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="match" type="6" refreshedVersion="3" background="1" saveData="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="match" type="6" refreshedVersion="3" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Datatables\match.csv" decimal="," thousands=" " comma="1">
       <textFields count="16">
         <textField/>
@@ -79,7 +85,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="matchday" type="6" refreshedVersion="3" background="1" saveData="1">
+  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="matchday" type="6" refreshedVersion="3" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Datatables\matchday.csv" decimal="," thousands=" " comma="1">
       <textFields count="4">
         <textField/>
@@ -428,8 +434,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -505,21 +511,21 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="matchday" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="matchday" connectionId="3" xr16:uid="{00000000-0016-0000-0400-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="club" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="club" connectionId="1" xr16:uid="{00000000-0016-0000-0600-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="match" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="match" connectionId="2" xr16:uid="{00000000-0016-0000-0D00-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -557,9 +563,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -591,9 +597,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -625,9 +649,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -800,14 +842,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
@@ -816,7 +858,7 @@
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -833,7 +875,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -854,19 +896,19 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -889,7 +931,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -915,20 +957,20 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -987,7 +1029,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1034,19 +1076,19 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1090,7 +1132,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1123,14 +1165,14 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
@@ -1140,7 +1182,7 @@
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1160,7 +1202,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1183,14 +1225,14 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -1210,7 +1252,7 @@
     <col min="16" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1260,7 +1302,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1289,16 +1331,16 @@
         <v>43</v>
       </c>
       <c r="L2" s="6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M2" s="5">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="O2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1327,16 +1369,16 @@
         <v>43</v>
       </c>
       <c r="L3" s="5">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="M3" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1365,16 +1407,16 @@
         <v>43</v>
       </c>
       <c r="L4" s="5">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="M4" s="5">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="O4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1403,7 +1445,7 @@
         <v>43</v>
       </c>
       <c r="L5" s="5">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="M5" s="5">
         <v>5</v>
@@ -1412,7 +1454,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1441,208 +1483,208 @@
         <v>43</v>
       </c>
       <c r="L6" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M6" s="5">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="O6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="2:3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="2:3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="2:3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="2:3">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="2:3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="2:3">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="2:3">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="2:3">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="2:3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="2:3">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="2:3">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="2:3">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="2:3">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
       <c r="C37" s="3"/>
     </row>
-    <row r="38" spans="2:3">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
       <c r="C38" s="3"/>
     </row>
-    <row r="39" spans="2:3">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
       <c r="C39" s="3"/>
     </row>
-    <row r="40" spans="2:3">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
       <c r="C40" s="3"/>
     </row>
-    <row r="41" spans="2:3">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="3"/>
     </row>
-    <row r="42" spans="2:3">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="3"/>
     </row>
-    <row r="43" spans="2:3">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="2:3">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" s="2"/>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" spans="2:3">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" s="2"/>
       <c r="C45" s="3"/>
     </row>
-    <row r="46" spans="2:3">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" s="2"/>
       <c r="C46" s="3"/>
     </row>
-    <row r="47" spans="2:3">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" spans="2:3">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
       <c r="C48" s="3"/>
     </row>
-    <row r="49" spans="2:3">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
       <c r="C49" s="3"/>
     </row>
-    <row r="50" spans="2:3">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
       <c r="C50" s="3"/>
     </row>
-    <row r="51" spans="2:3">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
       <c r="C51" s="3"/>
     </row>
-    <row r="52" spans="2:3">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="2"/>
       <c r="C52" s="3"/>
     </row>
-    <row r="53" spans="2:3">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" s="2"/>
       <c r="C53" s="3"/>
     </row>
-    <row r="54" spans="2:3">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" s="2"/>
       <c r="C54" s="3"/>
     </row>
-    <row r="55" spans="2:3">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" s="2"/>
       <c r="C55" s="3"/>
     </row>
@@ -1653,21 +1695,21 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1687,16 +1729,16 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1719,16 +1761,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1739,7 +1781,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1756,14 +1798,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -1772,7 +1814,7 @@
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1789,7 +1831,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1812,14 +1854,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
@@ -1827,7 +1869,7 @@
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1841,7 +1883,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1861,14 +1903,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
@@ -1876,7 +1918,7 @@
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1890,7 +1932,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1904,7 +1946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1918,7 +1960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1932,7 +1974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1946,7 +1988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1967,14 +2009,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -1996,7 +2038,7 @@
     <col min="19" max="19" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2055,7 +2097,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2102,14 +2144,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
@@ -2127,7 +2169,7 @@
     <col min="16" max="16" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2177,7 +2219,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2206,7 +2248,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2235,7 +2277,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2264,7 +2306,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2293,7 +2335,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2322,46 +2364,46 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="2:2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="2:2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="2:2">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="2:2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
     </row>
   </sheetData>
@@ -2370,14 +2412,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
@@ -2391,7 +2433,7 @@
     <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2426,7 +2468,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2455,14 +2497,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="18.140625" bestFit="1" customWidth="1"/>
@@ -2472,7 +2514,7 @@
     <col min="13" max="13" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2513,7 +2555,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2533,7 +2575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2553,7 +2595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2573,7 +2615,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2593,7 +2635,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Added ranking_by_series_id.sql and extra series in testdata
</commit_message>
<xml_diff>
--- a/tests/Testdata.xlsx
+++ b/tests/Testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maart\Documents\Syntra\groepswerk-1\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4874BE71-2BEC-44A3-BC27-3BE689F94685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDC03A1-C551-4B0B-BE57-984922369385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="844" firstSheet="1" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="844" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Season" sheetId="15" r:id="rId1"/>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="111">
   <si>
     <t>id</t>
   </si>
@@ -429,6 +429,9 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>Week 2</t>
   </si>
 </sst>
 </file>
@@ -1228,7 +1231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
@@ -1855,16 +1858,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1897,7 +1900,22 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>